<commit_message>
Modified Domino Flash SPI tile to fit a standard SPI Flash jig and SPI Flash chip footprint
</commit_message>
<xml_diff>
--- a/Domino JTAG SPI/BOM/Domino JTAG SPI BOM.xlsx
+++ b/Domino JTAG SPI/BOM/Domino JTAG SPI BOM.xlsx
@@ -11,28 +11,31 @@
     <sheet name="Domino JTAG SPI Rev. B" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>Item</t>
   </si>
@@ -61,34 +64,46 @@
     <t>Remarks</t>
   </si>
   <si>
+    <t>100n</t>
+  </si>
+  <si>
+    <t>ANY</t>
+  </si>
+  <si>
+    <t>C0402_100n_X7R_10%_CER_50V</t>
+  </si>
+  <si>
+    <t>C0402</t>
+  </si>
+  <si>
+    <t>C1, C3</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V 10% X7R 0402</t>
+  </si>
+  <si>
     <t>10n</t>
   </si>
   <si>
-    <t>ANY</t>
-  </si>
-  <si>
     <t>C0402_10n_X7R_10%_CER_50V</t>
   </si>
   <si>
-    <t>C0402</t>
-  </si>
-  <si>
-    <t>C1</t>
+    <t>C2</t>
   </si>
   <si>
     <t>CAP CER 10000PF 50V 10% X7R 0402</t>
   </si>
   <si>
-    <t>100n</t>
-  </si>
-  <si>
-    <t>C0402_100n_X7R_10%_CER_50V</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 50V 10% X7R 0402</t>
+    <t>MH8-1</t>
+  </si>
+  <si>
+    <t>MH8-1-0.1</t>
+  </si>
+  <si>
+    <t>J1, J5</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT .100 1ROW 8POS 8.08 HEAD 3.05 TAIL 15AU</t>
   </si>
   <si>
     <t>MH10-1</t>
@@ -97,7 +112,7 @@
     <t>MH10-1-0.1</t>
   </si>
   <si>
-    <t>J1, J2</t>
+    <t>J2, J3</t>
   </si>
   <si>
     <t>CONN HEADER VERT .100 1ROW 10POS 8.08 HEAD 3.05 TAIL 15AU</t>
@@ -109,28 +124,16 @@
     <t>MH2-1-0.1</t>
   </si>
   <si>
-    <t>J3</t>
+    <t>J4</t>
   </si>
   <si>
     <t>CONN HEADER VERT .100 1ROW 2POS 8.08 HEAD 3.05 TAIL 15AU</t>
   </si>
   <si>
-    <t>MH3-2</t>
-  </si>
-  <si>
-    <t>MH3-2-0.1</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT .100 2ROWS 3POS 8.08 HEAD 3.05 TAIL 15AU</t>
-  </si>
-  <si>
     <t>MHRA7-2-0.1</t>
   </si>
   <si>
-    <t>J5</t>
+    <t>J6</t>
   </si>
   <si>
     <t>CONN HEADER SHROUDED R/A .100 2ROWS 7POS 6.10 HEAD 3.05 TAIL 15AU</t>
@@ -145,7 +148,7 @@
     <t>R0402</t>
   </si>
   <si>
-    <t>R1, R2, R3, R5, R6</t>
+    <t>R1, R2, R3, R4, R6, R7</t>
   </si>
   <si>
     <t>RES 10K OHM 1/16W 5% 0402 SMD</t>
@@ -160,7 +163,7 @@
     <t>R0603</t>
   </si>
   <si>
-    <t>R4(DNP), R7(DNP), R8(DNP)</t>
+    <t>R5(DNP), R8(DNP), R9(DNP), R10, R11, R12, R13, R14(DNP)</t>
   </si>
   <si>
     <t>RES 0.0 OHM 1/8W JUMP SMD 0603</t>
@@ -176,6 +179,18 @@
   </si>
   <si>
     <t>SWITCH TACTILE SPST-NO 0.02A 15V</t>
+  </si>
+  <si>
+    <t>SPI_FLASH</t>
+  </si>
+  <si>
+    <t>SOIC-8</t>
+  </si>
+  <si>
+    <t>U1(DNP)</t>
+  </si>
+  <si>
+    <t>SPI FLASH SMD</t>
   </si>
 </sst>
 </file>
@@ -286,22 +301,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2:H11"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.83921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.2470588235294"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.0823529411765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.1686274509804"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.2470588235294"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.156862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.0274509803922"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5372549019608"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.77254901960784"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.90980392156863"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.6352941176471"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.5058823529412"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.6274509803922"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.6352941176471"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.7529411764706"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.7137254901961"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.90980392156863"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -338,7 +353,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>9</v>
@@ -416,7 +431,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>23</v>
@@ -494,7 +509,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>34</v>
@@ -520,7 +535,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>39</v>
@@ -565,6 +580,32 @@
       </c>
       <c r="H10" s="0" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added series resistors on SPI Flash SO in Domino JTAG SPI tile
</commit_message>
<xml_diff>
--- a/Domino JTAG SPI/BOM/Domino JTAG SPI BOM.xlsx
+++ b/Domino JTAG SPI/BOM/Domino JTAG SPI BOM.xlsx
@@ -11,31 +11,32 @@
     <sheet name="Domino JTAG SPI Rev. B" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>Item</t>
   </si>
@@ -139,16 +140,28 @@
     <t>CONN HEADER SHROUDED R/A .100 2ROWS 7POS 6.10 HEAD 3.05 TAIL 15AU</t>
   </si>
   <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>R0402_1k_5%_62.5mW</t>
+  </si>
+  <si>
+    <t>R0402</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>RES 1K OHM 1/16W 5% 0402 SMD</t>
+  </si>
+  <si>
     <t>10k</t>
   </si>
   <si>
     <t>R0402_10k_5%_62.5mW</t>
   </si>
   <si>
-    <t>R0402</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R4, R6, R7</t>
+    <t>R2, R3, R4, R5, R7, R8</t>
   </si>
   <si>
     <t>RES 10K OHM 1/16W 5% 0402 SMD</t>
@@ -163,7 +176,7 @@
     <t>R0603</t>
   </si>
   <si>
-    <t>R5(DNP), R8(DNP), R9(DNP), R10, R11, R12, R13, R14(DNP)</t>
+    <t>R6(DNP), R9(DNP), R10(DNP), R11, R12, R13, R14, R15(DNP)</t>
   </si>
   <si>
     <t>RES 0.0 OHM 1/8W JUMP SMD 0603</t>
@@ -301,22 +314,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2:H11"/>
+      <selection activeCell="C6" activeCellId="0" pane="topLeft" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.90980392156863"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.6352941176471"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.5058823529412"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.6274509803922"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.6352941176471"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.7529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.7137254901961"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6941176470588"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.90980392156863"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.92941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7725490196078"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.643137254902"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.7803921568627"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.7725490196078"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.9607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="70.0666666666667"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.95294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -509,7 +522,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>34</v>
@@ -535,7 +548,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>39</v>
@@ -547,13 +560,13 @@
         <v>40</v>
       </c>
       <c r="F9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
@@ -561,19 +574,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>46</v>
@@ -587,25 +600,51 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>48</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>48</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>50</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Domino JTAG SPI to Rev. C
</commit_message>
<xml_diff>
--- a/Domino JTAG SPI/BOM/Domino JTAG SPI BOM.xlsx
+++ b/Domino JTAG SPI/BOM/Domino JTAG SPI BOM.xlsx
@@ -8,28 +8,29 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino JTAG SPI Rev. B" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino JTAG SPI Rev. C" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -143,7 +144,7 @@
     <t>1k</t>
   </si>
   <si>
-    <t>R0402_1k_5%_62.5mW</t>
+    <t>R0402_0R_5%_62.5mW</t>
   </si>
   <si>
     <t>R0402</t>
@@ -152,7 +153,7 @@
     <t>R1</t>
   </si>
   <si>
-    <t>RES 1K OHM 1/16W 5% 0402 SMD</t>
+    <t>RES 0.0 OHM 1/16W JUMP 0402 SMD</t>
   </si>
   <si>
     <t>10k</t>
@@ -161,7 +162,7 @@
     <t>R0402_10k_5%_62.5mW</t>
   </si>
   <si>
-    <t>R2, R3, R4, R5, R7, R8</t>
+    <t>R2, R3, R4, R5, R7, R8, R16</t>
   </si>
   <si>
     <t>RES 10K OHM 1/16W 5% 0402 SMD</t>
@@ -317,19 +318,19 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C6" activeCellId="0" pane="topLeft" sqref="C6"/>
+      <selection activeCell="G10" activeCellId="0" pane="topLeft" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.92941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7725490196078"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.643137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.7803921568627"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.7725490196078"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.9607843137255"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="70.0666666666667"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.95294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.95686274509804"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.9058823529412"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7882352941176"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.9372549019608"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9058823529412"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="52.6823529411765"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="70.4196078431373"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -548,7 +549,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Domino JTAG SPI Rev. D: changed silkscreen font ratio to 20%
</commit_message>
<xml_diff>
--- a/Domino JTAG SPI/BOM/Domino JTAG SPI BOM.xlsx
+++ b/Domino JTAG SPI/BOM/Domino JTAG SPI BOM.xlsx
@@ -8,29 +8,30 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino JTAG SPI Rev. C" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino JTAG SPI Rev. D" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino JTAG SPI Rev. D'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -322,15 +323,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.95686274509804"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.9058823529412"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7882352941176"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.9372549019608"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9058823529412"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="52.6823529411765"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="70.4196078431373"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.9843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.043137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.0980392156863"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.043137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="52.9450980392157"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="70.7725490196078"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">

</xml_diff>